<commit_message>
removed hashmap of point values dataHM, findMin now works on both clouds, evaluation of point scores
</commit_message>
<xml_diff>
--- a/pcFilter.xlsx
+++ b/pcFilter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\IdeaProjects\pcFilter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411F95D4-88A0-4A61-BE82-E7E8909F7895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B834A6-4B2A-48C0-8BA2-F3CF23D0E703}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32640" yWindow="1665" windowWidth="23745" windowHeight="13980" xr2:uid="{741B5F6A-326F-49A4-94B6-A30D0DFC55CE}"/>
+    <workbookView xWindow="29685" yWindow="690" windowWidth="24600" windowHeight="13980" xr2:uid="{741B5F6A-326F-49A4-94B6-A30D0DFC55CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>stddevp_excel</t>
   </si>
@@ -75,12 +75,6 @@
     <t>std</t>
   </si>
   <si>
-    <t>normalized x</t>
-  </si>
-  <si>
-    <t>data (x)</t>
-  </si>
-  <si>
     <t>f1.txt</t>
   </si>
   <si>
@@ -97,6 +91,15 @@
   </si>
   <si>
     <t>abs(x - med)</t>
+  </si>
+  <si>
+    <t>P/L Intensity</t>
+  </si>
+  <si>
+    <t>NumberOfReturns</t>
+  </si>
+  <si>
+    <t>P/L Intensity (normalized)</t>
   </si>
 </sst>
 </file>
@@ -487,17 +490,18 @@
   <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.7109375" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.5703125" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.140625" customWidth="1"/>
     <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
@@ -506,7 +510,10 @@
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
@@ -527,30 +534,33 @@
         <v>5</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="U1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
         <v>0.7</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3" s="5">
         <f>_xlfn.STDEV.P(C3:C6)</f>
@@ -604,6 +614,9 @@
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C4" s="2">
         <v>1.2</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
       </c>
       <c r="E4" s="2"/>
       <c r="I4">
@@ -631,6 +644,9 @@
       <c r="C5" s="2">
         <v>1.3</v>
       </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="I5">
         <f>C5 - H3</f>
@@ -656,6 +672,9 @@
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <v>0.4</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
       </c>
       <c r="E6" s="2"/>
       <c r="I6">
@@ -695,7 +714,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>3.5</v>

</xml_diff>